<commit_message>
new model perf table
</commit_message>
<xml_diff>
--- a/Data/Predictions/SVM/SVM_Classifier_Predictions_All_Features_PCA.xlsx
+++ b/Data/Predictions/SVM/SVM_Classifier_Predictions_All_Features_PCA.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -2292,7 +2292,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -2400,7 +2400,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -2670,7 +2670,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -2751,7 +2751,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -2832,7 +2832,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -2994,7 +2994,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -3642,7 +3642,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -3696,7 +3696,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -4128,7 +4128,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -4371,7 +4371,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -4641,7 +4641,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -4668,7 +4668,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -4722,7 +4722,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -4830,7 +4830,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -4938,7 +4938,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -5100,7 +5100,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -5478,7 +5478,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -5991,7 +5991,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -6072,7 +6072,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -6126,7 +6126,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -6153,7 +6153,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -6207,7 +6207,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -6261,7 +6261,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -6504,7 +6504,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -6612,7 +6612,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -6639,7 +6639,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -6963,7 +6963,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -6990,7 +6990,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -7017,7 +7017,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -7044,7 +7044,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -7179,7 +7179,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -7206,7 +7206,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -7233,7 +7233,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -7260,7 +7260,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -7368,7 +7368,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -7395,7 +7395,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -7449,7 +7449,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -7476,7 +7476,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -7584,7 +7584,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -7665,7 +7665,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -7692,7 +7692,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -7881,7 +7881,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -7908,7 +7908,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -7935,7 +7935,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -8232,7 +8232,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -8259,7 +8259,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -8286,7 +8286,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -8340,7 +8340,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -8367,7 +8367,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -8394,7 +8394,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -8421,7 +8421,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -8475,7 +8475,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -8637,7 +8637,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -8664,7 +8664,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -8691,7 +8691,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -8799,7 +8799,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -8826,7 +8826,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -8853,7 +8853,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -8988,7 +8988,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -9123,7 +9123,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -9177,7 +9177,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -9312,7 +9312,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -9366,7 +9366,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -9501,7 +9501,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -9528,7 +9528,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -9609,7 +9609,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -9636,7 +9636,7 @@
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -9690,7 +9690,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -9717,7 +9717,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -9771,7 +9771,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -9798,7 +9798,7 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -10068,7 +10068,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -10149,7 +10149,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -10230,7 +10230,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -10257,7 +10257,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -10338,7 +10338,7 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -10365,7 +10365,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -10392,7 +10392,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -10473,7 +10473,7 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -10527,7 +10527,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -10554,7 +10554,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -10581,7 +10581,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -10608,7 +10608,7 @@
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -10662,7 +10662,7 @@
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -10716,7 +10716,7 @@
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -10797,7 +10797,7 @@
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -10878,7 +10878,7 @@
       </c>
       <c r="E387" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -10932,7 +10932,7 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -10959,7 +10959,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -10986,7 +10986,7 @@
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -11121,7 +11121,7 @@
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -11148,7 +11148,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -11256,7 +11256,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -11283,7 +11283,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -11445,7 +11445,7 @@
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -11472,7 +11472,7 @@
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -11499,7 +11499,7 @@
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -11580,7 +11580,7 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -11607,7 +11607,7 @@
       </c>
       <c r="E414" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -11634,7 +11634,7 @@
       </c>
       <c r="E415" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -11661,7 +11661,7 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -11688,7 +11688,7 @@
       </c>
       <c r="E417" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -11742,7 +11742,7 @@
       </c>
       <c r="E419" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -11769,7 +11769,7 @@
       </c>
       <c r="E420" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -11796,7 +11796,7 @@
       </c>
       <c r="E421" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -11850,7 +11850,7 @@
       </c>
       <c r="E423" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -11985,7 +11985,7 @@
       </c>
       <c r="E428" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -12066,7 +12066,7 @@
       </c>
       <c r="E431" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12120,7 +12120,7 @@
       </c>
       <c r="E433" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12174,7 +12174,7 @@
       </c>
       <c r="E435" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -12201,7 +12201,7 @@
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -12228,7 +12228,7 @@
       </c>
       <c r="E437" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -12255,7 +12255,7 @@
       </c>
       <c r="E438" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12282,7 +12282,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12309,7 +12309,7 @@
       </c>
       <c r="E440" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -12336,7 +12336,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12363,7 +12363,7 @@
       </c>
       <c r="E442" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12444,7 +12444,7 @@
       </c>
       <c r="E445" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -12471,7 +12471,7 @@
       </c>
       <c r="E446" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -12552,7 +12552,7 @@
       </c>
       <c r="E449" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12579,7 +12579,7 @@
       </c>
       <c r="E450" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12633,7 +12633,7 @@
       </c>
       <c r="E452" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -12687,7 +12687,7 @@
       </c>
       <c r="E454" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -12795,7 +12795,7 @@
       </c>
       <c r="E458" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12822,7 +12822,7 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -12849,7 +12849,7 @@
       </c>
       <c r="E460" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -12876,7 +12876,7 @@
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -12957,7 +12957,7 @@
       </c>
       <c r="E464" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -13146,7 +13146,7 @@
       </c>
       <c r="E471" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -13173,7 +13173,7 @@
       </c>
       <c r="E472" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -13227,7 +13227,7 @@
       </c>
       <c r="E474" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -13254,7 +13254,7 @@
       </c>
       <c r="E475" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -13281,7 +13281,7 @@
       </c>
       <c r="E476" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -13335,7 +13335,7 @@
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -13362,7 +13362,7 @@
       </c>
       <c r="E479" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -13443,7 +13443,7 @@
       </c>
       <c r="E482" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -13551,7 +13551,7 @@
       </c>
       <c r="E486" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -13632,7 +13632,7 @@
       </c>
       <c r="E489" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -13659,7 +13659,7 @@
       </c>
       <c r="E490" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -13713,7 +13713,7 @@
       </c>
       <c r="E492" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -13794,7 +13794,7 @@
       </c>
       <c r="E495" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -13821,7 +13821,7 @@
       </c>
       <c r="E496" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -13902,7 +13902,7 @@
       </c>
       <c r="E499" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -13929,7 +13929,7 @@
       </c>
       <c r="E500" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -14010,7 +14010,7 @@
       </c>
       <c r="E503" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -14118,7 +14118,7 @@
       </c>
       <c r="E507" t="inlineStr">
         <is>
-          <t>Convertible</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -14145,7 +14145,7 @@
       </c>
       <c r="E508" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -14253,7 +14253,7 @@
       </c>
       <c r="E512" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -14415,7 +14415,7 @@
       </c>
       <c r="E518" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -14442,7 +14442,7 @@
       </c>
       <c r="E519" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -14469,7 +14469,7 @@
       </c>
       <c r="E520" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -14496,7 +14496,7 @@
       </c>
       <c r="E521" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -14685,7 +14685,7 @@
       </c>
       <c r="E528" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -14712,7 +14712,7 @@
       </c>
       <c r="E529" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -14847,7 +14847,7 @@
       </c>
       <c r="E534" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -14874,7 +14874,7 @@
       </c>
       <c r="E535" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -14928,7 +14928,7 @@
       </c>
       <c r="E537" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -14955,7 +14955,7 @@
       </c>
       <c r="E538" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -15036,7 +15036,7 @@
       </c>
       <c r="E541" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -15063,7 +15063,7 @@
       </c>
       <c r="E542" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -15252,7 +15252,7 @@
       </c>
       <c r="E549" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -15279,7 +15279,7 @@
       </c>
       <c r="E550" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -15387,7 +15387,7 @@
       </c>
       <c r="E554" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -15441,7 +15441,7 @@
       </c>
       <c r="E556" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -15522,7 +15522,7 @@
       </c>
       <c r="E559" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -15549,7 +15549,7 @@
       </c>
       <c r="E560" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -15630,7 +15630,7 @@
       </c>
       <c r="E563" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -15711,7 +15711,7 @@
       </c>
       <c r="E566" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -15873,7 +15873,7 @@
       </c>
       <c r="E572" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -15927,7 +15927,7 @@
       </c>
       <c r="E574" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -16008,7 +16008,7 @@
       </c>
       <c r="E577" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -16089,7 +16089,7 @@
       </c>
       <c r="E580" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -16143,7 +16143,7 @@
       </c>
       <c r="E582" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -16170,7 +16170,7 @@
       </c>
       <c r="E583" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -16251,7 +16251,7 @@
       </c>
       <c r="E586" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -16413,7 +16413,7 @@
       </c>
       <c r="E592" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -16494,7 +16494,7 @@
       </c>
       <c r="E595" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -16575,7 +16575,7 @@
       </c>
       <c r="E598" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -16629,7 +16629,7 @@
       </c>
       <c r="E600" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -16683,7 +16683,7 @@
       </c>
       <c r="E602" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -16791,7 +16791,7 @@
       </c>
       <c r="E606" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -16845,7 +16845,7 @@
       </c>
       <c r="E608" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -16899,7 +16899,7 @@
       </c>
       <c r="E610" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -16953,7 +16953,7 @@
       </c>
       <c r="E612" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -17034,7 +17034,7 @@
       </c>
       <c r="E615" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -17088,7 +17088,7 @@
       </c>
       <c r="E617" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -17196,7 +17196,7 @@
       </c>
       <c r="E621" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -17304,7 +17304,7 @@
       </c>
       <c r="E625" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -17358,7 +17358,7 @@
       </c>
       <c r="E627" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -17493,7 +17493,7 @@
       </c>
       <c r="E632" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -17628,7 +17628,7 @@
       </c>
       <c r="E637" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -17655,7 +17655,7 @@
       </c>
       <c r="E638" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -17763,7 +17763,7 @@
       </c>
       <c r="E642" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -17844,7 +17844,7 @@
       </c>
       <c r="E645" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -17925,7 +17925,7 @@
       </c>
       <c r="E648" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -17952,7 +17952,7 @@
       </c>
       <c r="E649" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -18060,7 +18060,7 @@
       </c>
       <c r="E653" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -18141,7 +18141,7 @@
       </c>
       <c r="E656" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -18195,7 +18195,7 @@
       </c>
       <c r="E658" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -18303,7 +18303,7 @@
       </c>
       <c r="E662" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -18330,7 +18330,7 @@
       </c>
       <c r="E663" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -18438,7 +18438,7 @@
       </c>
       <c r="E667" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -18465,7 +18465,7 @@
       </c>
       <c r="E668" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -18519,7 +18519,7 @@
       </c>
       <c r="E670" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -18546,7 +18546,7 @@
       </c>
       <c r="E671" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -18573,7 +18573,7 @@
       </c>
       <c r="E672" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -18627,7 +18627,7 @@
       </c>
       <c r="E674" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -18843,7 +18843,7 @@
       </c>
       <c r="E682" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -18870,7 +18870,7 @@
       </c>
       <c r="E683" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -18924,7 +18924,7 @@
       </c>
       <c r="E685" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -19059,7 +19059,7 @@
       </c>
       <c r="E690" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -19086,7 +19086,7 @@
       </c>
       <c r="E691" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -19167,7 +19167,7 @@
       </c>
       <c r="E694" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -19194,7 +19194,7 @@
       </c>
       <c r="E695" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -19221,7 +19221,7 @@
       </c>
       <c r="E696" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -19248,7 +19248,7 @@
       </c>
       <c r="E697" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -19383,7 +19383,7 @@
       </c>
       <c r="E702" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -19491,7 +19491,7 @@
       </c>
       <c r="E706" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -19572,7 +19572,7 @@
       </c>
       <c r="E709" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -19626,7 +19626,7 @@
       </c>
       <c r="E711" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -19653,7 +19653,7 @@
       </c>
       <c r="E712" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -19788,7 +19788,7 @@
       </c>
       <c r="E717" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -19950,7 +19950,7 @@
       </c>
       <c r="E723" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -20058,7 +20058,7 @@
       </c>
       <c r="E727" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -20166,7 +20166,7 @@
       </c>
       <c r="E731" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -20274,7 +20274,7 @@
       </c>
       <c r="E735" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -20301,7 +20301,7 @@
       </c>
       <c r="E736" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -20328,7 +20328,7 @@
       </c>
       <c r="E737" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -20382,7 +20382,7 @@
       </c>
       <c r="E739" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -20490,7 +20490,7 @@
       </c>
       <c r="E743" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -20625,7 +20625,7 @@
       </c>
       <c r="E748" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -20706,7 +20706,7 @@
       </c>
       <c r="E751" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -20733,7 +20733,7 @@
       </c>
       <c r="E752" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -20868,7 +20868,7 @@
       </c>
       <c r="E757" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -20949,7 +20949,7 @@
       </c>
       <c r="E760" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -21030,7 +21030,7 @@
       </c>
       <c r="E763" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -21111,7 +21111,7 @@
       </c>
       <c r="E766" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -21138,7 +21138,7 @@
       </c>
       <c r="E767" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -21165,7 +21165,7 @@
       </c>
       <c r="E768" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -21516,7 +21516,7 @@
       </c>
       <c r="E781" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -21597,7 +21597,7 @@
       </c>
       <c r="E784" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -21624,7 +21624,7 @@
       </c>
       <c r="E785" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -21651,7 +21651,7 @@
       </c>
       <c r="E786" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -21813,7 +21813,7 @@
       </c>
       <c r="E792" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -21921,7 +21921,7 @@
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -22083,7 +22083,7 @@
       </c>
       <c r="E802" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -22245,7 +22245,7 @@
       </c>
       <c r="E808" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -22272,7 +22272,7 @@
       </c>
       <c r="E809" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -22299,7 +22299,7 @@
       </c>
       <c r="E810" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -22326,7 +22326,7 @@
       </c>
       <c r="E811" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -22380,7 +22380,7 @@
       </c>
       <c r="E813" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -22461,7 +22461,7 @@
       </c>
       <c r="E816" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -22488,7 +22488,7 @@
       </c>
       <c r="E817" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -22569,7 +22569,7 @@
       </c>
       <c r="E820" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -22731,7 +22731,7 @@
       </c>
       <c r="E826" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -22785,7 +22785,7 @@
       </c>
       <c r="E828" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -22893,7 +22893,7 @@
       </c>
       <c r="E832" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -23001,7 +23001,7 @@
       </c>
       <c r="E836" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -23028,7 +23028,7 @@
       </c>
       <c r="E837" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -23055,7 +23055,7 @@
       </c>
       <c r="E838" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -23136,7 +23136,7 @@
       </c>
       <c r="E841" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -23217,7 +23217,7 @@
       </c>
       <c r="E844" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -23244,7 +23244,7 @@
       </c>
       <c r="E845" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -23298,7 +23298,7 @@
       </c>
       <c r="E847" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -23352,7 +23352,7 @@
       </c>
       <c r="E849" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -23379,7 +23379,7 @@
       </c>
       <c r="E850" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -23460,7 +23460,7 @@
       </c>
       <c r="E853" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -23568,7 +23568,7 @@
       </c>
       <c r="E857" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -23622,7 +23622,7 @@
       </c>
       <c r="E859" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -23784,7 +23784,7 @@
       </c>
       <c r="E865" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -23811,7 +23811,7 @@
       </c>
       <c r="E866" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -23838,7 +23838,7 @@
       </c>
       <c r="E867" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -23946,7 +23946,7 @@
       </c>
       <c r="E871" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -24081,7 +24081,7 @@
       </c>
       <c r="E876" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -24135,7 +24135,7 @@
       </c>
       <c r="E878" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -24243,7 +24243,7 @@
       </c>
       <c r="E882" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -24432,7 +24432,7 @@
       </c>
       <c r="E889" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -24513,7 +24513,7 @@
       </c>
       <c r="E892" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -24540,7 +24540,7 @@
       </c>
       <c r="E893" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -24621,7 +24621,7 @@
       </c>
       <c r="E896" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -24675,7 +24675,7 @@
       </c>
       <c r="E898" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -24729,7 +24729,7 @@
       </c>
       <c r="E900" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -24810,7 +24810,7 @@
       </c>
       <c r="E903" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -24945,7 +24945,7 @@
       </c>
       <c r="E908" t="inlineStr">
         <is>
-          <t>Convertible</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -24972,7 +24972,7 @@
       </c>
       <c r="E909" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -24999,7 +24999,7 @@
       </c>
       <c r="E910" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -25323,7 +25323,7 @@
       </c>
       <c r="E922" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -25350,7 +25350,7 @@
       </c>
       <c r="E923" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -25431,7 +25431,7 @@
       </c>
       <c r="E926" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -25512,7 +25512,7 @@
       </c>
       <c r="E929" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -25566,7 +25566,7 @@
       </c>
       <c r="E931" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -25593,7 +25593,7 @@
       </c>
       <c r="E932" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -25674,7 +25674,7 @@
       </c>
       <c r="E935" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -25809,7 +25809,7 @@
       </c>
       <c r="E940" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -25836,7 +25836,7 @@
       </c>
       <c r="E941" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -25944,7 +25944,7 @@
       </c>
       <c r="E945" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -25998,7 +25998,7 @@
       </c>
       <c r="E947" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -26025,7 +26025,7 @@
       </c>
       <c r="E948" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -26052,7 +26052,7 @@
       </c>
       <c r="E949" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -26079,7 +26079,7 @@
       </c>
       <c r="E950" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -26133,7 +26133,7 @@
       </c>
       <c r="E952" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -26241,7 +26241,7 @@
       </c>
       <c r="E956" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -26322,7 +26322,7 @@
       </c>
       <c r="E959" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -26646,7 +26646,7 @@
       </c>
       <c r="E971" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -26781,7 +26781,7 @@
       </c>
       <c r="E976" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -26862,7 +26862,7 @@
       </c>
       <c r="E979" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -26916,7 +26916,7 @@
       </c>
       <c r="E981" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -26943,7 +26943,7 @@
       </c>
       <c r="E982" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -26997,7 +26997,7 @@
       </c>
       <c r="E984" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -27051,7 +27051,7 @@
       </c>
       <c r="E986" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -27213,7 +27213,7 @@
       </c>
       <c r="E992" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -27240,7 +27240,7 @@
       </c>
       <c r="E993" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -27348,7 +27348,7 @@
       </c>
       <c r="E997" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -27456,7 +27456,7 @@
       </c>
       <c r="E1001" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -27726,7 +27726,7 @@
       </c>
       <c r="E1011" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -27780,7 +27780,7 @@
       </c>
       <c r="E1013" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -27834,7 +27834,7 @@
       </c>
       <c r="E1015" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -27888,7 +27888,7 @@
       </c>
       <c r="E1017" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -28023,7 +28023,7 @@
       </c>
       <c r="E1022" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -28050,7 +28050,7 @@
       </c>
       <c r="E1023" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -28104,7 +28104,7 @@
       </c>
       <c r="E1025" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -28131,7 +28131,7 @@
       </c>
       <c r="E1026" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -28158,7 +28158,7 @@
       </c>
       <c r="E1027" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -28266,7 +28266,7 @@
       </c>
       <c r="E1031" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -28293,7 +28293,7 @@
       </c>
       <c r="E1032" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -28428,7 +28428,7 @@
       </c>
       <c r="E1037" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -28455,7 +28455,7 @@
       </c>
       <c r="E1038" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -28482,7 +28482,7 @@
       </c>
       <c r="E1039" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -28617,7 +28617,7 @@
       </c>
       <c r="E1044" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -28806,7 +28806,7 @@
       </c>
       <c r="E1051" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -28860,7 +28860,7 @@
       </c>
       <c r="E1053" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -28941,7 +28941,7 @@
       </c>
       <c r="E1056" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -28968,7 +28968,7 @@
       </c>
       <c r="E1057" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -28995,7 +28995,7 @@
       </c>
       <c r="E1058" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -29076,7 +29076,7 @@
       </c>
       <c r="E1061" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -29103,7 +29103,7 @@
       </c>
       <c r="E1062" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -29130,7 +29130,7 @@
       </c>
       <c r="E1063" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -29346,7 +29346,7 @@
       </c>
       <c r="E1071" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -29373,7 +29373,7 @@
       </c>
       <c r="E1072" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -29454,7 +29454,7 @@
       </c>
       <c r="E1075" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -29886,7 +29886,7 @@
       </c>
       <c r="E1091" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -29940,7 +29940,7 @@
       </c>
       <c r="E1093" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -30075,7 +30075,7 @@
       </c>
       <c r="E1098" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -30129,7 +30129,7 @@
       </c>
       <c r="E1100" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -30318,7 +30318,7 @@
       </c>
       <c r="E1107" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -30372,7 +30372,7 @@
       </c>
       <c r="E1109" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -30399,7 +30399,7 @@
       </c>
       <c r="E1110" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -30480,7 +30480,7 @@
       </c>
       <c r="E1113" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -30507,7 +30507,7 @@
       </c>
       <c r="E1114" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -30588,7 +30588,7 @@
       </c>
       <c r="E1117" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -30615,7 +30615,7 @@
       </c>
       <c r="E1118" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -30696,7 +30696,7 @@
       </c>
       <c r="E1121" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -30750,7 +30750,7 @@
       </c>
       <c r="E1123" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -30777,7 +30777,7 @@
       </c>
       <c r="E1124" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -30966,7 +30966,7 @@
       </c>
       <c r="E1131" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -31047,7 +31047,7 @@
       </c>
       <c r="E1134" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -31074,7 +31074,7 @@
       </c>
       <c r="E1135" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -31101,7 +31101,7 @@
       </c>
       <c r="E1136" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -31263,7 +31263,7 @@
       </c>
       <c r="E1142" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -31290,7 +31290,7 @@
       </c>
       <c r="E1143" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -31425,7 +31425,7 @@
       </c>
       <c r="E1148" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -31506,7 +31506,7 @@
       </c>
       <c r="E1151" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -31560,7 +31560,7 @@
       </c>
       <c r="E1153" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -31722,7 +31722,7 @@
       </c>
       <c r="E1159" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -31776,7 +31776,7 @@
       </c>
       <c r="E1161" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -31830,7 +31830,7 @@
       </c>
       <c r="E1163" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -31992,7 +31992,7 @@
       </c>
       <c r="E1169" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -32046,7 +32046,7 @@
       </c>
       <c r="E1171" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -32073,7 +32073,7 @@
       </c>
       <c r="E1172" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -32100,7 +32100,7 @@
       </c>
       <c r="E1173" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -32235,7 +32235,7 @@
       </c>
       <c r="E1178" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -32316,7 +32316,7 @@
       </c>
       <c r="E1181" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -32370,7 +32370,7 @@
       </c>
       <c r="E1183" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -32397,7 +32397,7 @@
       </c>
       <c r="E1184" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -32505,7 +32505,7 @@
       </c>
       <c r="E1188" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -32532,7 +32532,7 @@
       </c>
       <c r="E1189" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -32586,7 +32586,7 @@
       </c>
       <c r="E1191" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -32667,7 +32667,7 @@
       </c>
       <c r="E1194" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -32802,7 +32802,7 @@
       </c>
       <c r="E1199" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -32829,7 +32829,7 @@
       </c>
       <c r="E1200" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -32856,7 +32856,7 @@
       </c>
       <c r="E1201" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -33099,7 +33099,7 @@
       </c>
       <c r="E1210" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -33126,7 +33126,7 @@
       </c>
       <c r="E1211" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -33153,7 +33153,7 @@
       </c>
       <c r="E1212" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -33207,7 +33207,7 @@
       </c>
       <c r="E1214" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -33261,7 +33261,7 @@
       </c>
       <c r="E1216" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -33288,7 +33288,7 @@
       </c>
       <c r="E1217" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -33342,7 +33342,7 @@
       </c>
       <c r="E1219" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -33396,7 +33396,7 @@
       </c>
       <c r="E1221" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -33477,7 +33477,7 @@
       </c>
       <c r="E1224" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -33504,7 +33504,7 @@
       </c>
       <c r="E1225" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -33531,7 +33531,7 @@
       </c>
       <c r="E1226" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -33720,7 +33720,7 @@
       </c>
       <c r="E1233" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -33963,7 +33963,7 @@
       </c>
       <c r="E1242" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -33990,7 +33990,7 @@
       </c>
       <c r="E1243" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -34044,7 +34044,7 @@
       </c>
       <c r="E1245" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -34125,7 +34125,7 @@
       </c>
       <c r="E1248" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -34152,7 +34152,7 @@
       </c>
       <c r="E1249" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -34206,7 +34206,7 @@
       </c>
       <c r="E1251" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -34395,7 +34395,7 @@
       </c>
       <c r="E1258" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -34422,7 +34422,7 @@
       </c>
       <c r="E1259" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -34503,7 +34503,7 @@
       </c>
       <c r="E1262" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -34530,7 +34530,7 @@
       </c>
       <c r="E1263" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -34638,7 +34638,7 @@
       </c>
       <c r="E1267" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -34692,7 +34692,7 @@
       </c>
       <c r="E1269" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -34746,7 +34746,7 @@
       </c>
       <c r="E1271" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -34908,7 +34908,7 @@
       </c>
       <c r="E1277" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -34935,7 +34935,7 @@
       </c>
       <c r="E1278" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -34989,7 +34989,7 @@
       </c>
       <c r="E1280" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -35097,7 +35097,7 @@
       </c>
       <c r="E1284" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -35151,7 +35151,7 @@
       </c>
       <c r="E1286" t="inlineStr">
         <is>
-          <t>Convertible</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -35178,7 +35178,7 @@
       </c>
       <c r="E1287" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -35286,7 +35286,7 @@
       </c>
       <c r="E1291" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -35340,7 +35340,7 @@
       </c>
       <c r="E1293" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -35367,7 +35367,7 @@
       </c>
       <c r="E1294" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -35475,7 +35475,7 @@
       </c>
       <c r="E1298" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -35610,7 +35610,7 @@
       </c>
       <c r="E1303" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -35718,7 +35718,7 @@
       </c>
       <c r="E1307" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -35826,7 +35826,7 @@
       </c>
       <c r="E1311" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -35853,7 +35853,7 @@
       </c>
       <c r="E1312" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -35907,7 +35907,7 @@
       </c>
       <c r="E1314" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -35934,7 +35934,7 @@
       </c>
       <c r="E1315" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -35961,7 +35961,7 @@
       </c>
       <c r="E1316" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -35988,7 +35988,7 @@
       </c>
       <c r="E1317" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -36015,7 +36015,7 @@
       </c>
       <c r="E1318" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -36042,7 +36042,7 @@
       </c>
       <c r="E1319" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -36123,7 +36123,7 @@
       </c>
       <c r="E1322" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -36177,7 +36177,7 @@
       </c>
       <c r="E1324" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -36204,7 +36204,7 @@
       </c>
       <c r="E1325" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -36285,7 +36285,7 @@
       </c>
       <c r="E1328" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -36447,7 +36447,7 @@
       </c>
       <c r="E1334" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -36555,7 +36555,7 @@
       </c>
       <c r="E1338" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -36798,7 +36798,7 @@
       </c>
       <c r="E1347" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -36825,7 +36825,7 @@
       </c>
       <c r="E1348" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -36933,7 +36933,7 @@
       </c>
       <c r="E1352" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -36987,7 +36987,7 @@
       </c>
       <c r="E1354" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -37041,7 +37041,7 @@
       </c>
       <c r="E1356" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -37095,7 +37095,7 @@
       </c>
       <c r="E1358" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -37176,7 +37176,7 @@
       </c>
       <c r="E1361" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -37365,7 +37365,7 @@
       </c>
       <c r="E1368" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -37473,7 +37473,7 @@
       </c>
       <c r="E1372" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -37527,7 +37527,7 @@
       </c>
       <c r="E1374" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -37662,7 +37662,7 @@
       </c>
       <c r="E1379" t="inlineStr">
         <is>
-          <t>Pickup</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -37770,7 +37770,7 @@
       </c>
       <c r="E1383" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -37797,7 +37797,7 @@
       </c>
       <c r="E1384" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -37851,7 +37851,7 @@
       </c>
       <c r="E1386" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -37932,7 +37932,7 @@
       </c>
       <c r="E1389" t="inlineStr">
         <is>
-          <t>Convertible</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -37959,7 +37959,7 @@
       </c>
       <c r="E1390" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -38013,7 +38013,7 @@
       </c>
       <c r="E1392" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -38040,7 +38040,7 @@
       </c>
       <c r="E1393" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -38094,7 +38094,7 @@
       </c>
       <c r="E1395" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -38148,7 +38148,7 @@
       </c>
       <c r="E1397" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -38283,7 +38283,7 @@
       </c>
       <c r="E1402" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -38337,7 +38337,7 @@
       </c>
       <c r="E1404" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -38418,7 +38418,7 @@
       </c>
       <c r="E1407" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -38526,7 +38526,7 @@
       </c>
       <c r="E1411" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -38553,7 +38553,7 @@
       </c>
       <c r="E1412" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -38634,7 +38634,7 @@
       </c>
       <c r="E1415" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -38715,7 +38715,7 @@
       </c>
       <c r="E1418" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -38742,7 +38742,7 @@
       </c>
       <c r="E1419" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -38769,7 +38769,7 @@
       </c>
       <c r="E1420" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -38877,7 +38877,7 @@
       </c>
       <c r="E1424" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -38904,7 +38904,7 @@
       </c>
       <c r="E1425" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -39012,7 +39012,7 @@
       </c>
       <c r="E1429" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -39093,7 +39093,7 @@
       </c>
       <c r="E1432" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -39120,7 +39120,7 @@
       </c>
       <c r="E1433" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -39228,7 +39228,7 @@
       </c>
       <c r="E1437" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -39255,7 +39255,7 @@
       </c>
       <c r="E1438" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -39282,7 +39282,7 @@
       </c>
       <c r="E1439" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -39309,7 +39309,7 @@
       </c>
       <c r="E1440" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -39336,7 +39336,7 @@
       </c>
       <c r="E1441" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -39498,7 +39498,7 @@
       </c>
       <c r="E1447" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -39525,7 +39525,7 @@
       </c>
       <c r="E1448" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -39579,7 +39579,7 @@
       </c>
       <c r="E1450" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -39606,7 +39606,7 @@
       </c>
       <c r="E1451" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Sedan</t>
         </is>
       </c>
     </row>
@@ -39660,7 +39660,7 @@
       </c>
       <c r="E1453" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -39687,7 +39687,7 @@
       </c>
       <c r="E1454" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -39768,7 +39768,7 @@
       </c>
       <c r="E1457" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -39849,7 +39849,7 @@
       </c>
       <c r="E1460" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -39930,7 +39930,7 @@
       </c>
       <c r="E1463" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -39957,7 +39957,7 @@
       </c>
       <c r="E1464" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -40011,7 +40011,7 @@
       </c>
       <c r="E1466" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -40065,7 +40065,7 @@
       </c>
       <c r="E1468" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -40092,7 +40092,7 @@
       </c>
       <c r="E1469" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>Pickup</t>
         </is>
       </c>
     </row>
@@ -40470,7 +40470,7 @@
       </c>
       <c r="E1483" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -40551,7 +40551,7 @@
       </c>
       <c r="E1486" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>
@@ -40578,7 +40578,7 @@
       </c>
       <c r="E1487" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>Convertible</t>
         </is>
       </c>
     </row>
@@ -40659,7 +40659,7 @@
       </c>
       <c r="E1490" t="inlineStr">
         <is>
-          <t>Sedan</t>
+          <t>SUV</t>
         </is>
       </c>
     </row>

</xml_diff>